<commit_message>
Plot added to poster
</commit_message>
<xml_diff>
--- a/Documents/PSM Plots.xlsx
+++ b/Documents/PSM Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiern\Documents\GitHub\ModelingFinalProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59988F61-4EBD-4BEC-973C-0FE174B73537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58BAC36-A287-4ECB-BCE4-78884A9A35F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,6 +586,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PSM 5th</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Order Simulation with a Time Step of 1 Second</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27212775949112589"/>
+          <c:y val="1.183431585074598E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3762,6 +3800,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time step</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3803,6 +3901,8 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="20"/>
+        <c:tickMarkSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -3827,6 +3927,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance in</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> meters</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3870,37 +4030,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -4505,16 +4634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>133348</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4841,8 +4970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X510"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>